<commit_message>
Null values in legend - fixed
</commit_message>
<xml_diff>
--- a/documents/Published/CalendarVisual/CalendarVisualByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/CalendarVisual/CalendarVisualByMAQSoftwareChecklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SriramV\Desktop\Final build\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\documents\Published\CalendarVisual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19586C4C-BA76-481D-9350-9A60A03E5BC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D3980BF-082D-4609-BFFB-9468FC89B424}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{BBDE03C9-0260-4264-B62F-D02A960AE001}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{BBDE03C9-0260-4264-B62F-D02A960AE001}"/>
   </bookViews>
   <sheets>
     <sheet name="BVTs" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="149">
   <si>
     <t>Feature</t>
   </si>
@@ -591,6 +591,15 @@
 2.  If the end date time is not specified or Null, default time slot given for an event is 2 hours in the 'week view' and 'day view'.
 3. If start date time is same as end date time, in the 'list view' only start date is shown  
 4. If start date time is same as end date time, in the 'week view' and the 'day view', default time slot is given to the event which is 2 hours.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check if 'Event Group' has Blank value </t>
+  </si>
+  <si>
+    <t>1. Go to visual level filters and see if there is a blank value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The blank value should be reflected as Others in the Legends </t>
   </si>
 </sst>
 </file>
@@ -674,7 +683,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -742,6 +751,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1075,10 +1087,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{115B7480-3B3D-4922-96EC-1499616FB2AA}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1104,7 +1116,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="26" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1118,8 +1130,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
-      <c r="B4" s="24" t="s">
+      <c r="A4" s="26"/>
+      <c r="B4" s="25" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
@@ -1130,8 +1142,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
-      <c r="B5" s="24"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="25"/>
       <c r="C5" t="s">
         <v>138</v>
       </c>
@@ -1140,7 +1152,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
+      <c r="A6" s="26"/>
       <c r="B6" t="s">
         <v>139</v>
       </c>
@@ -1170,7 +1182,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="26" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
@@ -1184,7 +1196,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
+      <c r="A11" s="26"/>
       <c r="B11" t="s">
         <v>14</v>
       </c>
@@ -1196,7 +1208,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="4" t="s">
         <v>15</v>
       </c>
@@ -1208,7 +1220,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="4" t="s">
         <v>18</v>
       </c>
@@ -1231,349 +1243,366 @@
         <v>127</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="24"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D16" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B17" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
+    <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B19" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D19" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
-      <c r="B19" t="s">
+    <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="26"/>
+      <c r="B20" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C20" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
+    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B22" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D22" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
-      <c r="B22" s="7" t="s">
+    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="26"/>
+      <c r="B23" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D23" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="25"/>
-      <c r="B23" s="7" t="s">
+    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="26"/>
+      <c r="B24" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C24" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D24" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="25"/>
-      <c r="B24" s="7" t="s">
+    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="26"/>
+      <c r="B25" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D25" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="27" t="s">
+    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>88</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="25"/>
-      <c r="B27" t="s">
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="26"/>
+      <c r="B28" t="s">
         <v>89</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C28" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D28" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="25"/>
-      <c r="B28" t="s">
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="26"/>
+      <c r="B29" t="s">
         <v>90</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C29" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D29" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="25"/>
-      <c r="B29" t="s">
+    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="26"/>
+      <c r="B30" t="s">
         <v>91</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C30" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D30" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
+    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B32" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C32" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D32" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
-    </row>
-    <row r="33" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="12" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="12"/>
+    </row>
+    <row r="34" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B34" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C34" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D34" s="14" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
-      <c r="D34" s="14"/>
-    </row>
-    <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="25" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="12"/>
+      <c r="D35" s="14"/>
+    </row>
+    <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="B35" s="24" t="s">
+      <c r="B36" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C36" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D35" s="17" t="s">
+      <c r="D36" s="17" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="25"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="4" t="s">
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="26"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D37" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D37" s="14"/>
-    </row>
-    <row r="38" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" s="13" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="14"/>
+    </row>
+    <row r="39" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="B39" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C39" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D38" s="19" t="s">
+      <c r="D39" s="19" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
-      <c r="B39" s="14"/>
-      <c r="D39" s="14"/>
-    </row>
-    <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="13"/>
+      <c r="B40" s="14"/>
+      <c r="D40" s="14"/>
+    </row>
+    <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="B40" s="14" t="s">
+      <c r="B41" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C41" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D40" s="14" t="s">
+      <c r="D41" s="14" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="13"/>
-    </row>
-    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="13" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="13"/>
+    </row>
+    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="B42" s="14" t="s">
+      <c r="B43" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C43" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="D42" s="14" t="s">
+      <c r="D43" s="14" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="12" t="s">
+    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>116</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C45" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D45" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
-    </row>
-    <row r="46" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A46" s="25" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="12"/>
+    </row>
+    <row r="47" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A47" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="B46" s="24" t="s">
+      <c r="B47" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="C46" s="26" t="s">
+      <c r="C47" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="D47" s="4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A47" s="25"/>
-      <c r="B47" s="24"/>
-      <c r="C47" s="26"/>
-      <c r="D47" s="4" t="s">
+    <row r="48" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A48" s="26"/>
+      <c r="B48" s="25"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="4" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="25"/>
-      <c r="B48" s="24"/>
-      <c r="C48" s="26"/>
-      <c r="D48" s="4" t="s">
+    <row r="49" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A49" s="26"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="4" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="12"/>
-    </row>
-    <row r="50" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A50" s="12" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="12"/>
+    </row>
+    <row r="51" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>118</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C51" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="D51" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A52" s="12" t="s">
+    <row r="53" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A53" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B53" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C53" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D53" s="4" t="s">
         <v>133</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C46:C48"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="A27:A30"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="B46:B48"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="B47:B49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1583,7 +1612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{863B5848-521A-4A16-A6B0-43AE3145758E}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -1771,29 +1800,29 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="28">
+      <c r="A17" s="29">
         <v>16</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="30" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="28"/>
+      <c r="A18" s="29"/>
       <c r="B18" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="C18" s="29"/>
+      <c r="C18" s="30"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="28"/>
+      <c r="A19" s="29"/>
       <c r="B19" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="29"/>
+      <c r="C19" s="30"/>
     </row>
     <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
@@ -1807,41 +1836,41 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="28">
+      <c r="A21" s="29">
         <v>18</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="29" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="28"/>
+      <c r="A22" s="29"/>
       <c r="B22" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="C22" s="28"/>
+      <c r="C22" s="29"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="28"/>
+      <c r="A23" s="29"/>
       <c r="B23" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C23" s="28"/>
+      <c r="C23" s="29"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="28"/>
+      <c r="A24" s="29"/>
       <c r="B24" s="9"/>
-      <c r="C24" s="28"/>
+      <c r="C24" s="29"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="28"/>
+      <c r="A25" s="29"/>
       <c r="B25" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C25" s="28"/>
+      <c r="C25" s="29"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="9">

</xml_diff>

<commit_message>
FIxed legend interactivity after scroll, fixed legend color inconsistency, Upgraded API
</commit_message>
<xml_diff>
--- a/documents/Published/CalendarVisual/CalendarVisualByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/CalendarVisual/CalendarVisualByMAQSoftwareChecklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SriramV\Desktop\Final build\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VisualWork\documents\Published\CalendarVisual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19586C4C-BA76-481D-9350-9A60A03E5BC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A005AD47-F470-46B2-8F8B-4DB4959B3BCA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{BBDE03C9-0260-4264-B62F-D02A960AE001}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{BBDE03C9-0260-4264-B62F-D02A960AE001}"/>
   </bookViews>
   <sheets>
     <sheet name="BVTs" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="149">
   <si>
     <t>Feature</t>
   </si>
@@ -423,9 +423,6 @@
 </t>
   </si>
   <si>
-    <t>Work Days</t>
-  </si>
-  <si>
     <t>Check Active Work Days</t>
   </si>
   <si>
@@ -449,11 +446,6 @@
 2. Click Work Hours
 3. Select Start Time
 4. Select End Time</t>
-  </si>
-  <si>
-    <t>1. Click the format pane
-2. Click Work Days
-3. Toggle any of the days button.</t>
   </si>
   <si>
     <t xml:space="preserve">Current Time Line </t>
@@ -551,11 +543,6 @@
 cells not in specified time slot must gray out</t>
   </si>
   <si>
-    <t>1. Click on Format pane
-2. Click on Calendar Settings
-3. Select Week Strat Day from drop down box</t>
-  </si>
-  <si>
     <t>1. Add 'Date' in 'Start Date' Data bag
 2. Add 'Events' in Events databag</t>
   </si>
@@ -591,6 +578,28 @@
 2.  If the end date time is not specified or Null, default time slot given for an event is 2 hours in the 'week view' and 'day view'.
 3. If start date time is same as end date time, in the 'list view' only start date is shown  
 4. If start date time is same as end date time, in the 'week view' and the 'day view', default time slot is given to the event which is 2 hours.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check if 'Event Group' has Blank value </t>
+  </si>
+  <si>
+    <t>1. Go to visual level filters and see if there is a blank value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The blank value should be reflected as Others in the Legends </t>
+  </si>
+  <si>
+    <t>1. Click on Format pane
+2. Click on Calendar Settings
+3. Select Week Start Day from drop down box</t>
+  </si>
+  <si>
+    <t>Work week</t>
+  </si>
+  <si>
+    <t>1. Click the format pane
+2. Click Work week
+3. Toggle any of the days button.</t>
   </si>
 </sst>
 </file>
@@ -674,7 +683,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -744,16 +753,19 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1075,10 +1087,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{115B7480-3B3D-4922-96EC-1499616FB2AA}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1104,51 +1116,51 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="26" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
-      <c r="B4" s="24" t="s">
+      <c r="A4" s="26"/>
+      <c r="B4" s="28" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
-      <c r="B5" s="24"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="28"/>
       <c r="C5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
+      <c r="A6" s="26"/>
       <c r="B6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1157,20 +1169,20 @@
     </row>
     <row r="8" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="D8" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="B8" s="21" t="s">
-        <v>143</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>144</v>
-      </c>
-      <c r="D8" s="22" t="s">
-        <v>145</v>
-      </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="26" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
@@ -1184,7 +1196,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
+      <c r="A11" s="26"/>
       <c r="B11" t="s">
         <v>14</v>
       </c>
@@ -1196,7 +1208,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="4" t="s">
         <v>15</v>
       </c>
@@ -1208,7 +1220,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="4" t="s">
         <v>18</v>
       </c>
@@ -1222,360 +1234,378 @@
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="C14" s="4" t="s">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="24"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D16" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="C17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="26"/>
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="26"/>
+      <c r="B23" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="26"/>
+      <c r="B24" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="26"/>
+      <c r="B25" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" t="s">
+        <v>88</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="26"/>
+      <c r="B28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="26"/>
+      <c r="B29" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="26"/>
+      <c r="B30" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="12"/>
+    </row>
+    <row r="34" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
-      <c r="B19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
-      <c r="B22" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="25"/>
-      <c r="B23" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="25"/>
-      <c r="B24" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="27" t="s">
+      <c r="C34" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="12"/>
+      <c r="D35" s="14"/>
+    </row>
+    <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="B36" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="26"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="14"/>
+    </row>
+    <row r="39" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="13"/>
+      <c r="B40" s="14"/>
+      <c r="D40" s="14"/>
+    </row>
+    <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="13"/>
+    </row>
+    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="B26" t="s">
-        <v>88</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D26" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="25"/>
-      <c r="B27" t="s">
-        <v>89</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D27" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="25"/>
-      <c r="B28" t="s">
-        <v>90</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D28" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="25"/>
-      <c r="B29" t="s">
-        <v>91</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D29" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D31" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
-    </row>
-    <row r="33" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
-      <c r="D34" s="14"/>
-    </row>
-    <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="B35" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D35" s="17" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="25"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D36" s="3" t="s">
+      <c r="B43" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D43" s="14" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D37" s="14"/>
-    </row>
-    <row r="38" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="B38" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="C38" s="4" t="s">
+    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="D38" s="19" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
-      <c r="B39" s="14"/>
-      <c r="D39" s="14"/>
-    </row>
-    <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="B40" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="C40" s="4" t="s">
+      <c r="B45" t="s">
+        <v>114</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D45" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="12"/>
+    </row>
+    <row r="47" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A47" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="D40" s="14" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="13"/>
-    </row>
-    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="B42" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="D42" s="14" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="B44" t="s">
-        <v>116</v>
-      </c>
-      <c r="C44" s="4" t="s">
+      <c r="B47" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="C47" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="D44" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
-    </row>
-    <row r="46" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A46" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="B46" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="C46" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A47" s="25"/>
-      <c r="B47" s="24"/>
-      <c r="C47" s="26"/>
       <c r="D47" s="4" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="25"/>
-      <c r="B48" s="24"/>
-      <c r="C48" s="26"/>
+    <row r="48" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A48" s="26"/>
+      <c r="B48" s="28"/>
+      <c r="C48" s="25"/>
       <c r="D48" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A49" s="26"/>
+      <c r="B49" s="28"/>
+      <c r="C49" s="25"/>
+      <c r="D49" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="12"/>
+    </row>
+    <row r="51" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="B51" t="s">
+        <v>116</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D51" s="4" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="12"/>
-    </row>
-    <row r="50" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A50" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="B50" t="s">
-        <v>118</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A52" s="12" t="s">
+    <row r="53" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A53" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C53" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="D53" s="4" t="s">
         <v>131</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>133</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C46:C48"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="A26:A29"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="B46:B48"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="A27:A30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1583,7 +1613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{863B5848-521A-4A16-A6B0-43AE3145758E}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -1771,29 +1801,29 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="28">
+      <c r="A17" s="29">
         <v>16</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="30" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="28"/>
+      <c r="A18" s="29"/>
       <c r="B18" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="C18" s="29"/>
+      <c r="C18" s="30"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="28"/>
+      <c r="A19" s="29"/>
       <c r="B19" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="29"/>
+      <c r="C19" s="30"/>
     </row>
     <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
@@ -1807,41 +1837,41 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="28">
+      <c r="A21" s="29">
         <v>18</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="29" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="28"/>
+      <c r="A22" s="29"/>
       <c r="B22" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="C22" s="28"/>
+      <c r="C22" s="29"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="28"/>
+      <c r="A23" s="29"/>
       <c r="B23" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C23" s="28"/>
+      <c r="C23" s="29"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="28"/>
+      <c r="A24" s="29"/>
       <c r="B24" s="9"/>
-      <c r="C24" s="28"/>
+      <c r="C24" s="29"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="28"/>
+      <c r="A25" s="29"/>
       <c r="B25" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C25" s="28"/>
+      <c r="C25" s="29"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
@@ -1873,5 +1903,6 @@
     <mergeCell ref="C21:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Deleted typings.json Updated checklist
</commit_message>
<xml_diff>
--- a/documents/Published/CalendarVisual/CalendarVisualByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/CalendarVisual/CalendarVisualByMAQSoftwareChecklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VisualWork\documents\Published\CalendarVisual\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-saviss\source\repos\PowerBI-visuals2\documents\Published\CalendarVisual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A005AD47-F470-46B2-8F8B-4DB4959B3BCA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D0A11B-8C2B-486B-B3C8-D39FA2139F3B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{BBDE03C9-0260-4264-B62F-D02A960AE001}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BBDE03C9-0260-4264-B62F-D02A960AE001}"/>
   </bookViews>
   <sheets>
     <sheet name="BVTs" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="146">
   <si>
     <t>Feature</t>
   </si>
@@ -150,14 +150,6 @@
   <si>
     <t>1. Click on Format Pane
 2. Click on Events tab
-3. Toggle 'Month' Button</t>
-  </si>
-  <si>
-    <t>The 'Month' button should be displayed on the top right side above the table</t>
-  </si>
-  <si>
-    <t>1. Click on Format Pane
-2. Click on Events tab
 3. Toggle 'Week' Button</t>
   </si>
   <si>
@@ -169,9 +161,6 @@
     <t>1. Click on Format Pane
 2. Click on Events tab
 3. Toggle 'List' Button</t>
-  </si>
-  <si>
-    <t>Show Month Button</t>
   </si>
   <si>
     <t>Show Week Button</t>
@@ -580,15 +569,6 @@
 4. If start date time is same as end date time, in the 'week view' and the 'day view', default time slot is given to the event which is 2 hours.</t>
   </si>
   <si>
-    <t xml:space="preserve">Check if 'Event Group' has Blank value </t>
-  </si>
-  <si>
-    <t>1. Go to visual level filters and see if there is a blank value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The blank value should be reflected as Others in the Legends </t>
-  </si>
-  <si>
     <t>1. Click on Format pane
 2. Click on Calendar Settings
 3. Select Week Start Day from drop down box</t>
@@ -600,6 +580,16 @@
     <t>1. Click the format pane
 2. Click Work week
 3. Toggle any of the days button.</t>
+  </si>
+  <si>
+    <t>Change months using the &lt;&gt; keys</t>
+  </si>
+  <si>
+    <t>The Next or Previous 'Month' should be displayed and the visual shouldn't get stuck in an infinite loop for those months</t>
+  </si>
+  <si>
+    <t>1. Click on 'Month' Button
+2.Click '&lt;' or '&gt;' several times a bit faster</t>
   </si>
 </sst>
 </file>
@@ -756,16 +746,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1087,10 +1077,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{115B7480-3B3D-4922-96EC-1499616FB2AA}">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1123,7 +1113,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>6</v>
@@ -1131,11 +1121,11 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="26"/>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="25" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>7</v>
@@ -1143,9 +1133,9 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="26"/>
-      <c r="B5" s="28"/>
+      <c r="B5" s="25"/>
       <c r="C5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>7</v>
@@ -1154,13 +1144,13 @@
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="26"/>
       <c r="B6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C6" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1169,16 +1159,16 @@
     </row>
     <row r="8" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="D8" s="22" t="s">
         <v>139</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>140</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>141</v>
-      </c>
-      <c r="D8" s="22" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1234,13 +1224,13 @@
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1249,116 +1239,119 @@
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="B16" s="4" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="D16" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C17" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D16" s="4" t="s">
         <v>23</v>
       </c>
     </row>
+    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
     <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>26</v>
+      <c r="A19" s="26"/>
+      <c r="B19" t="s">
+        <v>28</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
-      <c r="B20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D19" t="s">
         <v>31</v>
       </c>
     </row>
+    <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
     <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
-        <v>32</v>
-      </c>
+      <c r="A22" s="26"/>
       <c r="B22" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="26"/>
       <c r="B23" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D23" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="26"/>
+    </row>
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
-      <c r="B24" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D24" s="6" t="s">
+      <c r="D25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D26" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="26"/>
+      <c r="B27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="26"/>
-      <c r="B25" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="B27" t="s">
-        <v>88</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>45</v>
       </c>
       <c r="D27" t="s">
         <v>47</v>
@@ -1367,242 +1360,230 @@
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="26"/>
       <c r="B28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="26"/>
       <c r="B29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="12"/>
+    </row>
+    <row r="33" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D29" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="26"/>
-      <c r="B30" t="s">
-        <v>91</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D30" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D32" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
-    </row>
-    <row r="34" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="12" t="s">
+      <c r="B33" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="12"/>
+      <c r="D34" s="14"/>
+    </row>
+    <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="B35" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="12"/>
-      <c r="D35" s="14"/>
-    </row>
-    <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="B36" s="28" t="s">
-        <v>92</v>
-      </c>
+      <c r="D35" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="26"/>
+      <c r="B36" s="25"/>
       <c r="C36" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D36" s="17" t="s">
+      <c r="D36" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="26"/>
-      <c r="B37" s="28"/>
-      <c r="C37" s="4" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="14"/>
+    </row>
+    <row r="38" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A38" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D38" s="19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="13"/>
+      <c r="B39" s="14"/>
+      <c r="D39" s="14"/>
+    </row>
+    <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="13"/>
+    </row>
+    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B42" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D38" s="14"/>
-    </row>
-    <row r="39" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="B39" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="C39" s="4" t="s">
+      <c r="C42" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B44" t="s">
+        <v>111</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D44" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="12"/>
+    </row>
+    <row r="46" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A46" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="B46" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="C46" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A47" s="26"/>
+      <c r="B47" s="25"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="26"/>
+      <c r="B48" s="25"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="12"/>
+    </row>
+    <row r="50" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="D39" s="19" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="13"/>
-      <c r="B40" s="14"/>
-      <c r="D40" s="14"/>
-    </row>
-    <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="B41" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="D41" s="14" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="13"/>
-    </row>
-    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="B43" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="D43" s="14" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="B45" t="s">
-        <v>114</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="D45" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="12"/>
-    </row>
-    <row r="47" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A47" s="26" t="s">
+      <c r="B50" t="s">
+        <v>113</v>
+      </c>
+      <c r="C50" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B47" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="C47" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A48" s="26"/>
-      <c r="B48" s="28"/>
-      <c r="C48" s="25"/>
-      <c r="D48" s="4" t="s">
+      <c r="D50" s="4" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A49" s="26"/>
-      <c r="B49" s="28"/>
-      <c r="C49" s="25"/>
-      <c r="D49" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="12"/>
-    </row>
-    <row r="51" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A51" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="B51" t="s">
-        <v>116</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A53" s="12" t="s">
+    <row r="52" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D52" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>131</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C46:C48"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A26:A29"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="B46:B48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1626,13 +1607,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1640,10 +1621,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1651,10 +1632,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1662,10 +1643,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1673,10 +1654,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1684,10 +1665,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1695,10 +1676,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1706,10 +1687,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1717,10 +1698,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1728,10 +1709,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1739,10 +1720,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1750,10 +1731,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1761,10 +1742,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1772,10 +1753,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1783,10 +1764,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1794,10 +1775,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1805,23 +1786,23 @@
         <v>16</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="29"/>
       <c r="B18" s="11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C18" s="30"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="29"/>
       <c r="B19" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C19" s="30"/>
     </row>
@@ -1830,10 +1811,10 @@
         <v>17</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1841,23 +1822,23 @@
         <v>18</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="29"/>
       <c r="B22" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C22" s="29"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="29"/>
       <c r="B23" s="9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C23" s="29"/>
     </row>
@@ -1869,7 +1850,7 @@
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="29"/>
       <c r="B25" s="9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C25" s="29"/>
     </row>
@@ -1878,10 +1859,10 @@
         <v>19</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1889,10 +1870,10 @@
         <v>20</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>